<commit_message>
Fix part_list to load all columns dynamically
</commit_message>
<xml_diff>
--- a/output/user_stage2_output.xlsx
+++ b/output/user_stage2_output.xlsx
@@ -1192,10 +1192,10 @@
     <t>[{"source_system": "pos", "source_file": "po_mock_newparts.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Aluminum Bracket 25x11 mm"}]</t>
   </si>
   <si>
-    <t>[{"source_system": "pos", "source_file": "po_mock_newparts.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Steel Screw 39x90 mm"}]</t>
-  </si>
-  <si>
-    <t>[{"source_system": "pos", "source_file": "po_mock_newparts.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Aluminum Washer 19x142 mm"}]</t>
+    <t>[{"source_system": "pos", "source_file": "po_mock_newparts.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Steel Screw 39x90 mm"}]</t>
+  </si>
+  <si>
+    <t>[{"source_system": "pos", "source_file": "po_mock_newparts.pdf"}, {"source_system": "user", "source_file": "diagram 3.pdf"}, {"source_system": "user", "source_file": "diagram 3.pdf"}, {"source_system": "user", "source_file": "diagram 3.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Aluminum Washer 19x142 mm"}]</t>
   </si>
   <si>
     <t>[{"source_system": "invoices", "source_file": "invoice_mock_newparts.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Aluminum Coupler 12x91 mm"}]</t>
@@ -1935,7 +1935,7 @@
         <v>60</v>
       </c>
       <c r="C2" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="K2" t="s">
         <v>124</v>
@@ -1997,7 +1997,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.56353754582</v>
       </c>
       <c r="K3" t="s">
         <v>125</v>
@@ -2056,7 +2056,7 @@
         <v>62</v>
       </c>
       <c r="C4" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.59985385615</v>
       </c>
       <c r="K4" t="s">
         <v>126</v>
@@ -2118,7 +2118,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.60609446955</v>
       </c>
       <c r="K5" t="s">
         <v>127</v>
@@ -2177,7 +2177,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="K6" t="s">
         <v>128</v>
@@ -2236,7 +2236,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="K7" t="s">
         <v>129</v>
@@ -2298,7 +2298,7 @@
         <v>66</v>
       </c>
       <c r="C8" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="K8" t="s">
         <v>130</v>
@@ -2360,7 +2360,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="K9" t="s">
         <v>131</v>
@@ -2422,7 +2422,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="K10" t="s">
         <v>132</v>
@@ -2484,7 +2484,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="K11" t="s">
         <v>133</v>
@@ -2546,7 +2546,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D12" t="s">
         <v>80</v>
@@ -2698,7 +2698,7 @@
         <v>71</v>
       </c>
       <c r="C13" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D13" t="s">
         <v>81</v>
@@ -2850,7 +2850,7 @@
         <v>72</v>
       </c>
       <c r="C14" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D14" t="s">
         <v>82</v>
@@ -2999,7 +2999,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D15" t="s">
         <v>83</v>
@@ -3151,7 +3151,7 @@
         <v>74</v>
       </c>
       <c r="C16" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D16" t="s">
         <v>84</v>
@@ -3309,7 +3309,7 @@
         <v>75</v>
       </c>
       <c r="C17" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D17" t="s">
         <v>85</v>
@@ -3464,7 +3464,7 @@
         <v>76</v>
       </c>
       <c r="C18" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D18" t="s">
         <v>86</v>
@@ -3610,7 +3610,7 @@
         <v>77</v>
       </c>
       <c r="C19" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D19" t="s">
         <v>87</v>
@@ -3765,7 +3765,7 @@
         <v>78</v>
       </c>
       <c r="C20" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D20" t="s">
         <v>88</v>
@@ -3917,7 +3917,7 @@
         <v>79</v>
       </c>
       <c r="C21" s="2">
-        <v>46000.70576734132</v>
+        <v>46001.95226143338</v>
       </c>
       <c r="D21" t="s">
         <v>89</v>

</xml_diff>